<commit_message>
Version one paper done
</commit_message>
<xml_diff>
--- a/Papers/Parallel/ResultIndividuals.xlsx
+++ b/Papers/Parallel/ResultIndividuals.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Emad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Emad\Source\Repos\Thesis Codes\SigmaNEAT\Papers\Parallel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBEC4B1-8142-43B1-AAC9-528DDD9778FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33AA7C-D790-4C6E-991B-64B2527ED0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6EBF8CA3-ECBB-4BD2-8BDE-65DB7F6EF012}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6EBF8CA3-ECBB-4BD2-8BDE-65DB7F6EF012}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Chart2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="IndivSingle" sheetId="3" r:id="rId1"/>
+    <sheet name="IndivTotal" sheetId="2" r:id="rId2"/>
+    <sheet name="Indiv" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -182,6 +182,860 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>GPU Per Individual Time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="41275" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Indiv!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Indiv!$M$2:$M$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>98.12866666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.759</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.964666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.210666666666668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.585999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.019333333333336</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.425333333333334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.274999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.454666666666668</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.485666666666667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.00333333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.444000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.091999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.650333333333332</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.233666666666668</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30.981999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.722333333333335</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30.582999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.457999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.158666666666665</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30.263999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>29.960999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>29.724333333333334</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29.772666666666666</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29.52</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29.456666666666667</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29.400333333333332</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.507333333333332</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.285666666666668</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.172333333333334</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28.992999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28.949333333333332</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>29.093666666666667</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28.825666666666667</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>28.923333333333332</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>28.817333333333334</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>28.856333333333332</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>28.823666666666668</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>28.582000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>28.503666666666668</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>28.424666666666667</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>28.501666666666665</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>28.416333333333334</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>28.379333333333335</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>28.356666666666666</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>28.366</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>28.337666666666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>28.308</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>28.344999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5E71-407C-9F46-44075F7BAF64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CPU Per Individual Time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="41275" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Indiv!$Q$2:$Q$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>63.144666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.334666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.545333333333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.50333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.700333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56.57033333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.68333333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55.015666666666668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.792000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.50033333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.397333333333336</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52.298333333333332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56.325333333333333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.886666666666663</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50.030999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>52.204333333333331</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>52.398333333333333</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50.924666666666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52.413333333333334</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54.279000000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>53.920333333333332</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>53.497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53.530333333333331</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>54.04</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>51.36933333333333</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>53.682333333333332</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>51.408999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>53.651666666666664</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>51.746000000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>53.526666666666664</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>51.957000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>53.68266666666667</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>53.534999999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>51.398000000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>51.50333333333333</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>51.585333333333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>53.301666666666669</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>53.040333333333336</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>53.359333333333332</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>55.438000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>51.201666666666668</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>53.297666666666665</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>53.368333333333332</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>53.00333333333333</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>53.072333333333333</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>49.597000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>52.981666666666669</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>51.148000000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>51.410666666666664</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>51.175666666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5E71-407C-9F46-44075F7BAF64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="820173135"/>
+        <c:axId val="626535839"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="820173135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Number of individuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="626535839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="626535839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Average time for a single individual training in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="820173135"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
             <c:v>GPU Total Time</c:v>
           </c:tx>
           <c:spPr>
@@ -198,7 +1052,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Indiv!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -357,7 +1211,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$51</c:f>
+              <c:f>Indiv!$E$2:$E$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -555,7 +1409,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>Indiv!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -714,7 +1568,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$51</c:f>
+              <c:f>Indiv!$I$2:$I$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -1136,860 +1990,6 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>GPU Per Individual Time</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="41275" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>370</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>390</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>420</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>430</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>440</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>450</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>470</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>490</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$M$2:$M$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>98.12866666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60.759</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>48.964666666666666</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44.210666666666668</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>38.585999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>38.019333333333336</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36.425333333333334</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.274999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34.454666666666668</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33.485666666666667</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>33.00333333333333</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32.444000000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>32.091999999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>31.650333333333332</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>31.233666666666668</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>30.981999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30.722333333333335</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30.582999999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>30.457999999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30.158666666666665</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>30.263999999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>29.960999999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>29.724333333333334</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>29.772666666666666</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>29.52</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>29.456666666666667</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>29.400333333333332</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>29.507333333333332</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29.285666666666668</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.172333333333334</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>28.992999999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>28.949333333333332</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>29.093666666666667</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>28.825666666666667</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>28.923333333333332</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>28.817333333333334</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>28.856333333333332</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>28.823666666666668</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>28.582000000000001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>28.7</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>28.503666666666668</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>28.424666666666667</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>28.501666666666665</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>28.416333333333334</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>28.379333333333335</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>28.356666666666666</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>28.366</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>28.337666666666667</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>28.308</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>28.344999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5E71-407C-9F46-44075F7BAF64}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>CPU Per Individual Time</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="41275" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>63.144666666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>61.334666666666664</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56.545333333333332</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>57.50333333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>54.700333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56.57033333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>55.68333333333333</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55.015666666666668</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>54.792000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50.50033333333333</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>54.397333333333336</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>52.298333333333332</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>56.325333333333333</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>55.886666666666663</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>50.030999999999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>52.204333333333331</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>52.398333333333333</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>50.924666666666667</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>52.413333333333334</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>54.279000000000003</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>53.920333333333332</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>53.497</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>53.530333333333331</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>54.04</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>51.36933333333333</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>53.682333333333332</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>51.408999999999999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>53.651666666666664</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>51.746000000000002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53.526666666666664</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>51.957000000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>53.68266666666667</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>53.534999999999997</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>51.398000000000003</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>51.50333333333333</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>51.585333333333331</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>53.301666666666669</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>53.040333333333336</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>53.359333333333332</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>55.438000000000002</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>51.201666666666668</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>53.297666666666665</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>53.368333333333332</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>53.00333333333333</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>53.072333333333333</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>49.597000000000001</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>52.981666666666669</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>51.148000000000003</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>51.410666666666664</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>51.175666666666665</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5E71-407C-9F46-44075F7BAF64}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="820173135"/>
-        <c:axId val="626535839"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="820173135"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Number of individuals</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="626535839"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="626535839"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Average time for a single individual training in milliseconds</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="820173135"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3157,10 +3157,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6DFE77B9-57A3-4511-9B5B-E9FBEE267B96}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A4AD84D0-2AB4-4827-A193-6F04DF0B4565}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3168,10 +3168,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A4AD84D0-2AB4-4827-A193-6F04DF0B4565}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6DFE77B9-57A3-4511-9B5B-E9FBEE267B96}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3188,7 +3188,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E725D9BD-4D36-411D-B9DF-437FE1FC307E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9158C627-4307-4172-A9A3-CE0A63AD3CAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3221,7 +3221,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9158C627-4307-4172-A9A3-CE0A63AD3CAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E725D9BD-4D36-411D-B9DF-437FE1FC307E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3544,7 +3544,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>